<commit_message>
Correct config of multiregion Excel file
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/multiregion_macro_input.xlsx
+++ b/message_ix/tests/data/multiregion_macro_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF58AB80-9635-4009-B3D0-0578D1384A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17D849-1112-4D96-A1B7-D4848AD36EED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="345" windowWidth="21600" windowHeight="12360" tabRatio="992" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="555" windowWidth="16200" windowHeight="12195" tabRatio="992" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>

</xml_diff>